<commit_message>
hw5 and hw4 solutions
</commit_message>
<xml_diff>
--- a/Homework/Homework 5/tcs94_ECHE313_HW5.xlsx
+++ b/Homework/Homework 5/tcs94_ECHE313_HW5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0f4dc847ec8b5479/Documents/CWRU/Spring 2025/ECHE313/Homework/Homework 5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="33" documentId="8_{9FDDEC87-E007-4932-A024-84C71EBE875F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{798928ED-B4D9-4A42-B0B4-211B8299D7E7}"/>
+  <xr:revisionPtr revIDLastSave="99" documentId="8_{9FDDEC87-E007-4932-A024-84C71EBE875F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C98BC3CC-299A-4F1E-9350-2B60DE8A274F}"/>
   <bookViews>
-    <workbookView xWindow="1520" yWindow="1520" windowWidth="19200" windowHeight="11170" xr2:uid="{EABE0706-3F5E-4B57-A7F8-40DA46E7CAA1}"/>
+    <workbookView xWindow="7320" yWindow="6360" windowWidth="28800" windowHeight="15285" xr2:uid="{EABE0706-3F5E-4B57-A7F8-40DA46E7CAA1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Catalyst 1</t>
   </si>
@@ -51,6 +51,18 @@
   </si>
   <si>
     <t>Std Dev</t>
+  </si>
+  <si>
+    <t>STD</t>
+  </si>
+  <si>
+    <t>AVG</t>
+  </si>
+  <si>
+    <t>BAR 1</t>
+  </si>
+  <si>
+    <t>BAR 2</t>
   </si>
 </sst>
 </file>
@@ -131,6 +143,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Mean Active</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Concentration Among Two Catalysts</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -172,7 +214,9 @@
           <c:order val="0"/>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:schemeClr val="accent4">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -185,54 +229,49 @@
             <c:errValType val="cust"/>
             <c:noEndCap val="0"/>
             <c:plus>
-              <c:numLit>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-              </c:numLit>
+              <c:numRef>
+                <c:f>Sheet1!$G$7:$G$8</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>3.44</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2.2200000000000002</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
             </c:plus>
             <c:minus>
-              <c:numLit>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-              </c:numLit>
+              <c:numRef>
+                <c:f>Sheet1!$G$7:$G$8</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>3.44</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2.2200000000000002</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
             </c:minus>
             <c:spPr>
               <a:noFill/>
               <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
                 <a:round/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
           </c:errBars>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$1:$B$1</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>Catalyst 1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Catalyst 2</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$A$14:$B$14</c:f>
+              <c:f>Sheet1!$F$7:$F$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -247,7 +286,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-A823-47ED-93A1-6AD456723134}"/>
+              <c16:uniqueId val="{00000000-3E20-4FCB-B1BA-400EA43302DB}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -261,18 +300,76 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="2120514431"/>
-        <c:axId val="1235137792"/>
+        <c:axId val="1607299471"/>
+        <c:axId val="1607298991"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2120514431"/>
+        <c:axId val="1607299471"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Catalyst</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Number</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
@@ -308,7 +405,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1235137792"/>
+        <c:crossAx val="1607298991"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -316,7 +413,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1235137792"/>
+        <c:axId val="1607298991"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -336,8 +433,71 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Active</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Concentration (g/L)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
@@ -367,7 +527,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2120514431"/>
+        <c:crossAx val="1607299471"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -395,12 +555,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -970,23 +1125,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>107950</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Chart 6">
+        <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4679B78A-4550-E91B-B820-76585AB05382}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{85FA28BD-E912-1834-A0D5-EAF946BFB1AF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1004,7 +1159,264 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>466726</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>161926</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="5" name="TextBox 4">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7CE95FD0-FFEE-E6F8-6270-0E821C08E03B}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="6562726" y="5162550"/>
+              <a:ext cx="4572000" cy="1371600"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+            <a:ln w="9525" cmpd="sng">
+              <a:noFill/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>Mean</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" baseline="0"/>
+                <a:t> active concentration of liquid laundry detergent based on two different catalyst types. </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>Data are represented as the mean </a:t>
+              </a:r>
+              <a14:m>
+                <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:r>
+                    <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                    </a:rPr>
+                    <m:t>±</m:t>
+                  </m:r>
+                </m:oMath>
+              </a14:m>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t> standard deviation with n = 1. (*) represents p &lt; 0.05 compared to the</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" baseline="0"/>
+                <a:t> second catalyst's</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t> performance,</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" baseline="0"/>
+                <a:t> using a two-sided, t-sample z-test in Minitab and by-hand with known population standard deviation of 3 g/L. We have sufficient evidence to reject the claim that the two catalysts yield the same concentrations, and accept that the concentration is dependent on catalyst choice.</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="5" name="TextBox 4">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7CE95FD0-FFEE-E6F8-6270-0E821C08E03B}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="6562726" y="5162550"/>
+              <a:ext cx="4572000" cy="1371600"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+            <a:ln w="9525" cmpd="sng">
+              <a:noFill/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>Mean</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" baseline="0"/>
+                <a:t> active concentration of liquid laundry detergent based on two different catalyst types. </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>Data are represented as the mean </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>±</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t> standard deviation with n = 1. (*) represents p &lt; 0.05 compared to the</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" baseline="0"/>
+                <a:t> second catalyst's</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t> performance,</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" baseline="0"/>
+                <a:t> using a two-sided, t-sample z-test in Minitab and by-hand with known population standard deviation of 3 g/L. We have sufficient evidence to reject the claim that the two catalysts yield the same concentrations, and accept that the concentration is dependent on catalyst choice.</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>104774</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="TextBox 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C56E612-BBE3-EBA6-ABBA-AC2885DC7EBB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7962900" y="3152774"/>
+          <a:ext cx="523875" cy="561975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>*</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1324,15 +1736,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10633FA7-7306-4038-8F7C-F97F754105BA}">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1340,7 +1752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>57.9</v>
       </c>
@@ -1348,7 +1760,7 @@
         <v>66.400000000000006</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>66.2</v>
       </c>
@@ -1356,7 +1768,7 @@
         <v>71.7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>65.400000000000006</v>
       </c>
@@ -1364,7 +1776,7 @@
         <v>70.3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>65.400000000000006</v>
       </c>
@@ -1372,31 +1784,55 @@
         <v>69.3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>65.2</v>
       </c>
       <c r="B6" s="1">
         <v>64.8</v>
       </c>
+      <c r="F6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>62.6</v>
       </c>
       <c r="B7" s="1">
         <v>69.599999999999994</v>
       </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7">
+        <v>65.22</v>
+      </c>
+      <c r="G7">
+        <v>3.44</v>
+      </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>67.599999999999994</v>
       </c>
       <c r="B8" s="1">
         <v>68.599999999999994</v>
       </c>
+      <c r="E8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8">
+        <v>68.42</v>
+      </c>
+      <c r="G8">
+        <v>2.2200000000000002</v>
+      </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>63.7</v>
       </c>
@@ -1404,7 +1840,7 @@
         <v>69.400000000000006</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>67.2</v>
       </c>
@@ -1412,7 +1848,7 @@
         <v>65.3</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>71</v>
       </c>
@@ -1420,13 +1856,13 @@
         <v>68.8</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B13" s="2"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>65.22</v>
       </c>
@@ -1434,13 +1870,13 @@
         <v>68.42</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B15" s="2"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>3.44</v>
       </c>
@@ -1448,13 +1884,13 @@
         <v>2.2200000000000002</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B17" s="2"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1.0892200000000001</v>
       </c>

</xml_diff>